<commit_message>
5-Se agregan los nuevos procedimientos aa la vitacora de la experiencia 2 y se da por finalizada
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -9,14 +9,17 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgRUJIRtO6w6kZ9Gffvuu/2tWVdww=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mib4cqr80cJk0l9AKSaJVhTwzK4QA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+  <si>
+    <t>EXPERIENCIA 1</t>
+  </si>
   <si>
     <t>Equipo</t>
   </si>
@@ -68,12 +71,45 @@
   <si>
     <t>Luego de hacer los ultimos cambios generales  y de responsive se da por terminado las primera expericiencia 1</t>
   </si>
+  <si>
+    <t>EXPERIENCIA 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mejoras y cambios a las páginas anteriores del proyecto </t>
+  </si>
+  <si>
+    <t>Implementacion del primer formulario de registro de datos</t>
+  </si>
+  <si>
+    <t>Se agregan las validaciones al formulario registro con java script</t>
+  </si>
+  <si>
+    <t>Se modifican los ultimos cambios y se da por terminado el formulario anterior</t>
+  </si>
+  <si>
+    <t>Se crea la segunda página llamada login la cúal esta destinada para el inicio de sesión pos registro</t>
+  </si>
+  <si>
+    <t>Se agregan interacciones y cambios de colores con el mouse al momento de pasar por encima del texto y al usar el botón entrar</t>
+  </si>
+  <si>
+    <t>Se crea un tercer formulario el cúal esta destinado para el uso de contacto y de comunicación con el sitio web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se agregan sus respectivas validaciones y se da por terminado </t>
+  </si>
+  <si>
+    <t>Se Vinculan las nuevas paginsa al sitio web para su facil acceso</t>
+  </si>
+  <si>
+    <t>Luego de hacer los ultimos cambios generales  y responsive se da por terminado la expericiencia 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -84,6 +120,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <b/>
       <sz val="14.0"/>
@@ -95,6 +132,17 @@
     </font>
     <font>
       <sz val="14.0"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,34 +173,43 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,163 +438,162 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2">
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+    </row>
+    <row r="4">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
         <v>11.0</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3">
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4">
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="B5" s="8"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="9">
+    </row>
+    <row r="9">
+      <c r="B9" s="4">
         <v>1.0</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="9">
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="4">
         <v>2.0</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="9">
+    </row>
+    <row r="11">
+      <c r="B11" s="4">
         <v>3.0</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="9">
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="4">
         <v>4.0</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="9">
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="4">
         <v>5.0</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="9">
+      <c r="C13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="4">
         <v>6.0</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="9">
+      <c r="C14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="4">
         <v>7.0</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="9">
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="4">
         <v>8.0</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="9">
+      <c r="C16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="4">
         <v>9.0</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="9">
+      <c r="C17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="4">
         <v>10.0</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="1"/>
+      <c r="C18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="1"/>
@@ -547,54 +603,165 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="1"/>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="1"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="1"/>
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="11">
+        <v>12.0</v>
+      </c>
+      <c r="D23" s="12"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="1"/>
+      <c r="B24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="1"/>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="12"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="1"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="1"/>
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="1"/>
+      <c r="B28" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="1"/>
+      <c r="B29" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="1"/>
+      <c r="B30" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="1"/>
+      <c r="B31" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="1"/>
+      <c r="B32" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="1"/>
+      <c r="B33" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="1"/>
+      <c r="B34" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="1"/>
+      <c r="B35" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="1"/>
+      <c r="B36" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="1"/>
+      <c r="B37" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="1"/>

</xml_diff>